<commit_message>
added Eagle Schematic V1
</commit_message>
<xml_diff>
--- a/AR0134CS/Capstone_AR0134CS_BOM.xlsx
+++ b/AR0134CS/Capstone_AR0134CS_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/447eb0fe645bf98e/Documents/GitHub/Capstone-Sightline/AR0134CS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kimba\OneDrive\Documents\GitHub\Capstone-Sightline\AR0134CS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="317" documentId="8_{D9F634DA-45E3-429E-AAAF-3B5973463A8B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{0A36DA94-DA48-475D-889F-20583B13F472}"/>
+  <xr:revisionPtr revIDLastSave="319" documentId="8_{D9F634DA-45E3-429E-AAAF-3B5973463A8B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{1EEA4395-16B8-4227-9FEF-DF87A872BFA8}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -1010,8 +1010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C17" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>